<commit_message>
feat: add tech files, delete wrong comments, correct migrations
</commit_message>
<xml_diff>
--- a/storage/test.xlsx
+++ b/storage/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Тестирование Авито\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8647FBD0-44E2-4FF1-93E0-C0835FF6C25E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F23132-FA4B-4C09-A9B4-7457598C4321}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>offer_id</t>
   </si>
@@ -55,30 +55,6 @@
   </si>
   <si>
     <t>computer</t>
-  </si>
-  <si>
-    <t>motherboard</t>
-  </si>
-  <si>
-    <t>CPU</t>
-  </si>
-  <si>
-    <t>GPU</t>
-  </si>
-  <si>
-    <t>RAM</t>
-  </si>
-  <si>
-    <t>Cables</t>
-  </si>
-  <si>
-    <t>Monitor</t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
 </sst>
 </file>
@@ -117,10 +93,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -402,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,19 +394,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -442,10 +418,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="2">
-        <v>15000</v>
+        <v>100000</v>
       </c>
       <c r="D2" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -459,13 +435,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>3000</v>
+        <v>12000</v>
       </c>
       <c r="D3" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -476,7 +452,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="2">
-        <v>7500</v>
+        <v>15000</v>
       </c>
       <c r="D4" s="1">
         <v>5</v>
@@ -493,131 +469,12 @@
         <v>7</v>
       </c>
       <c r="C5" s="2">
-        <v>1500</v>
+        <v>3200</v>
       </c>
       <c r="D5" s="1">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>10004</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2">
-        <v>12000</v>
-      </c>
-      <c r="D6" s="1">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>10005</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2">
-        <v>45000</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>10006</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2">
-        <v>90000</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>10007</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2">
-        <v>25000</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>10008</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1500</v>
-      </c>
-      <c r="D10" s="1">
-        <v>12</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10009</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2">
-        <v>42000</v>
-      </c>
-      <c r="D11" s="1">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10010</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2">
-        <v>11500</v>
-      </c>
-      <c r="D12" s="1">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>